<commit_message>
Added more no. of test cases
</commit_message>
<xml_diff>
--- a/testData/OpenCart-TestCases.xlsx
+++ b/testData/OpenCart-TestCases.xlsx
@@ -3,14 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java_Selenium\OpenCart_HybridFramework\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EA7BFE-7B64-4B6B-9F08-B04716668347}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{FD79D42D-C8E3-47D3-9F6E-C4B4586D5B65}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" tabRatio="914" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="6615" tabRatio="914" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vesion History" sheetId="2" r:id="rId1"/>
@@ -51,6 +46,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Register!$A$1:$K$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <oleSize ref="A1:F3"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -9898,8 +9894,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20598,7 +20594,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -23258,8 +23254,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -23986,8 +23982,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24388,8 +24384,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="A3" zoomScale="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25168,8 +25164,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25867,8 +25863,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26625,7 +26621,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="85" workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>

</xml_diff>